<commit_message>
Investigation into mobile simulator test executions
</commit_message>
<xml_diff>
--- a/Data Files/Search_Data_Mobile.xlsx
+++ b/Data Files/Search_Data_Mobile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A90980-CE13-47B0-B42A-33607F34A5E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1365247D-18E2-4FA5-BE81-AF0692903D80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>Tree Surgeon</t>
   </si>
@@ -163,6 +163,33 @@
   </si>
   <si>
     <t>Garage/Vehicle Services &gt; Diagnostic Testing</t>
+  </si>
+  <si>
+    <t>Emulation</t>
+  </si>
+  <si>
+    <t>{"CHROME_DRIVER":{}}</t>
+  </si>
+  <si>
+    <t>Addendum</t>
+  </si>
+  <si>
+    <t>Last row resets the file back to the default condition</t>
+  </si>
+  <si>
+    <t>{"CHROME_DRIVER":{"mobileEmulation":{"deviceName":"iPhone X"}}}</t>
+  </si>
+  <si>
+    <t>,"orientation":"LANDSCAPE"</t>
+  </si>
+  <si>
+    <t>{"CHROME_DRIVER":{"mobileEmulation":{"deviceName":"Galaxy S5"}}}</t>
+  </si>
+  <si>
+    <t>{"CHROME_DRIVER":{"mobileEmulation":{"deviceName":"iPad"}}}</t>
+  </si>
+  <si>
+    <t>{"CHROME_DRIVER":{"mobileEmulation":{"deviceName":Pixel 2 XL"}}}</t>
   </si>
 </sst>
 </file>
@@ -198,11 +225,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D56B88-33E9-468B-853E-05EE5D8A6600}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,9 +563,10 @@
     <col min="8" max="8" width="53.5703125" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="93.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -568,8 +597,14 @@
       <c r="J1" t="s">
         <v>38</v>
       </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -600,8 +635,14 @@
       <c r="J2">
         <v>800</v>
       </c>
+      <c r="K2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -632,8 +673,11 @@
       <c r="J3">
         <v>1000</v>
       </c>
+      <c r="K3" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -664,8 +708,11 @@
       <c r="J4">
         <v>900</v>
       </c>
+      <c r="K4" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -696,8 +743,11 @@
       <c r="J5">
         <v>600</v>
       </c>
+      <c r="K5" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -727,6 +777,12 @@
       </c>
       <c r="J6">
         <v>700</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>